<commit_message>
added most recent data and figures
</commit_message>
<xml_diff>
--- a/yeast_replaceable_genes/sequences/all_other_mendelian/dataAugust12.xlsx
+++ b/yeast_replaceable_genes/sequences/all_other_mendelian/dataAugust12.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="25360" windowHeight="16520" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="4160" windowWidth="25360" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="198">
   <si>
     <t>Gene</t>
   </si>
@@ -571,6 +571,48 @@
   </si>
   <si>
     <t>Fully conserved mutations</t>
+  </si>
+  <si>
+    <t>KIF1B</t>
+  </si>
+  <si>
+    <t>KIF5A</t>
+  </si>
+  <si>
+    <t>LARGE</t>
+  </si>
+  <si>
+    <t>LBR</t>
+  </si>
+  <si>
+    <t>hmzdy</t>
+  </si>
+  <si>
+    <t>LFNG</t>
+  </si>
+  <si>
+    <t>LIPA</t>
+  </si>
+  <si>
+    <t>LMAN1</t>
+  </si>
+  <si>
+    <t>LMNA</t>
+  </si>
+  <si>
+    <t>LRPPRC</t>
+  </si>
+  <si>
+    <t>LYST</t>
+  </si>
+  <si>
+    <t>MAGT1</t>
+  </si>
+  <si>
+    <t>MAN2B1</t>
+  </si>
+  <si>
+    <t>MANBA</t>
   </si>
 </sst>
 </file>
@@ -710,7 +752,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -738,6 +780,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -816,7 +864,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="480">
+  <cellStyleXfs count="550">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1297,8 +1345,78 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1371,8 +1489,12 @@
     <xf numFmtId="11" fontId="18" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="480">
+  <cellStyles count="550">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1612,6 +1734,41 @@
     <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="501" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="503" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="505" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="507" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="509" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1851,6 +2008,41 @@
     <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="500" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="502" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="504" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="506" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="508" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="510" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2181,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN134"/>
+  <dimension ref="A1:AN147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AM6" sqref="AM6"/>
+    <sheetView tabSelected="1" topLeftCell="G118" workbookViewId="0">
+      <selection activeCell="AG146" sqref="AG146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2509,7 +2701,7 @@
         <v>33</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG66" si="1">AVERAGE(AA3,AC3,AE3)</f>
+        <f t="shared" ref="AG3:AG65" si="1">AVERAGE(AA3,AC3,AE3)</f>
         <v>2.9233045333333336E-6</v>
       </c>
       <c r="AH3" s="3">
@@ -9777,7 +9969,7 @@
         <v>7.6084450000000001E-3</v>
       </c>
       <c r="AG68">
-        <f t="shared" ref="AG67:AG130" si="2">AVERAGE(AA68,AC68,AE68)</f>
+        <f t="shared" ref="AG68:AG128" si="2">AVERAGE(AA68,AC68,AE68)</f>
         <v>9.3317554999999996E-2</v>
       </c>
       <c r="AH68" s="27">
@@ -16871,284 +17063,1625 @@
       </c>
     </row>
     <row r="132" spans="1:37">
-      <c r="A132" s="1" t="s">
+      <c r="A132" s="72" t="s">
+        <v>184</v>
+      </c>
+      <c r="B132" s="27">
+        <v>0.72626611900000004</v>
+      </c>
+      <c r="C132" s="29">
+        <v>0.69989333300000001</v>
+      </c>
+      <c r="D132" s="27">
+        <v>0.78869999999999996</v>
+      </c>
+      <c r="E132" s="27">
+        <v>0.665418073</v>
+      </c>
+      <c r="F132" s="29">
+        <v>0.61154333299999997</v>
+      </c>
+      <c r="G132" s="27">
+        <v>0.80335999999999996</v>
+      </c>
+      <c r="H132" s="27">
+        <v>3.2050656329999998</v>
+      </c>
+      <c r="I132" s="36">
+        <v>3.286413333</v>
+      </c>
+      <c r="J132" s="27">
+        <v>4.7468300000000001</v>
+      </c>
+      <c r="K132" s="27">
+        <v>4</v>
+      </c>
+      <c r="L132" s="27">
+        <v>1</v>
+      </c>
+      <c r="M132" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="N132" s="27">
+        <v>1</v>
+      </c>
+      <c r="O132" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="P132" s="28">
+        <v>1.4E-3</v>
+      </c>
+      <c r="Q132" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="R132" s="27">
+        <v>0.112486302</v>
+      </c>
+      <c r="S132" s="27">
+        <v>0.118573425</v>
+      </c>
+      <c r="T132" s="27">
+        <v>0</v>
+      </c>
+      <c r="U132" s="27">
+        <v>0.246248889</v>
+      </c>
+      <c r="V132" s="27">
+        <v>0.28724095599999999</v>
+      </c>
+      <c r="W132" s="27">
+        <v>0</v>
+      </c>
+      <c r="X132" s="27">
+        <v>1.7320947310000001</v>
+      </c>
+      <c r="Y132" s="27">
+        <v>1.458075228</v>
+      </c>
+      <c r="Z132" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="36">
+        <v>0.368679443</v>
+      </c>
+      <c r="AB132" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC132" s="36">
+        <v>0.38812542999999999</v>
+      </c>
+      <c r="AD132" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE132" s="29">
+        <v>0.465955016</v>
+      </c>
+      <c r="AF132" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG132" s="72"/>
+      <c r="AH132" s="73"/>
+      <c r="AI132" s="73"/>
+      <c r="AJ132" s="73"/>
+      <c r="AK132" s="73"/>
+    </row>
+    <row r="133" spans="1:37">
+      <c r="A133" s="72" t="s">
+        <v>185</v>
+      </c>
+      <c r="B133" s="27">
+        <v>0.73189674400000004</v>
+      </c>
+      <c r="C133" s="27">
+        <v>0.79793199999999997</v>
+      </c>
+      <c r="D133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E133" s="27">
+        <v>0.642705843</v>
+      </c>
+      <c r="F133" s="27">
+        <v>0.83290299999999995</v>
+      </c>
+      <c r="G133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H133" s="27">
+        <v>3.2030907270000002</v>
+      </c>
+      <c r="I133" s="27">
+        <v>4.4197810000000004</v>
+      </c>
+      <c r="J133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K133" s="27">
+        <v>10</v>
+      </c>
+      <c r="L133" s="27">
+        <v>0</v>
+      </c>
+      <c r="M133" s="28">
+        <v>0</v>
+      </c>
+      <c r="N133" s="27">
+        <v>7</v>
+      </c>
+      <c r="O133" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="P133" s="28">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="Q133" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="R133" s="27">
+        <v>0.10511651299999999</v>
+      </c>
+      <c r="S133" s="27">
+        <v>9.1529544000000004E-2</v>
+      </c>
+      <c r="T133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U133" s="27">
+        <v>0.26104797000000002</v>
+      </c>
+      <c r="V133" s="27">
+        <v>0.27839491599999999</v>
+      </c>
+      <c r="W133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="X133" s="27">
+        <v>1.554072839</v>
+      </c>
+      <c r="Y133" s="27">
+        <v>1.47477244</v>
+      </c>
+      <c r="Z133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA133" s="31">
+        <v>2.4801729000000002E-2</v>
+      </c>
+      <c r="AB133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC133" s="31">
+        <v>2.9955017E-2</v>
+      </c>
+      <c r="AD133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE133" s="31">
+        <v>1.4488338999999999E-2</v>
+      </c>
+      <c r="AF133" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG133" s="72"/>
+      <c r="AH133" s="73"/>
+      <c r="AI133" s="73"/>
+      <c r="AJ133" s="73"/>
+      <c r="AK133" s="73"/>
+    </row>
+    <row r="134" spans="1:37">
+      <c r="A134" s="72" t="s">
+        <v>186</v>
+      </c>
+      <c r="B134" s="27">
+        <v>0.72571502600000004</v>
+      </c>
+      <c r="C134" s="36">
+        <v>0.76885000000000003</v>
+      </c>
+      <c r="D134" s="27">
+        <v>0.77344999999999997</v>
+      </c>
+      <c r="E134" s="27">
+        <v>0.58834505299999995</v>
+      </c>
+      <c r="F134" s="27">
+        <v>0.60326000000000002</v>
+      </c>
+      <c r="G134" s="27">
+        <v>0.44046000000000002</v>
+      </c>
+      <c r="H134" s="27">
+        <v>2.8661265340000002</v>
+      </c>
+      <c r="I134" s="27">
+        <v>3.357272</v>
+      </c>
+      <c r="J134" s="27">
+        <v>2.0487899999999999</v>
+      </c>
+      <c r="K134" s="27">
+        <v>6</v>
+      </c>
+      <c r="L134" s="27">
+        <v>1</v>
+      </c>
+      <c r="M134" s="28">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="N134" s="27">
+        <v>1</v>
+      </c>
+      <c r="O134" s="28">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="P134" s="28">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="Q134" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="R134" s="27">
+        <v>0.10064461700000001</v>
+      </c>
+      <c r="S134" s="27">
+        <v>5.0387545999999998E-2</v>
+      </c>
+      <c r="T134" s="27">
+        <v>0</v>
+      </c>
+      <c r="U134" s="27">
+        <v>0.203562565</v>
+      </c>
+      <c r="V134" s="27">
+        <v>0.13152716</v>
+      </c>
+      <c r="W134" s="27">
+        <v>0</v>
+      </c>
+      <c r="X134" s="27">
+        <v>1.5161377620000001</v>
+      </c>
+      <c r="Y134" s="27">
+        <v>1.831007077</v>
+      </c>
+      <c r="Z134" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA134" s="29">
+        <v>6.5916970000000005E-2</v>
+      </c>
+      <c r="AB134" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC134" s="29">
+        <v>0.40688074099999999</v>
+      </c>
+      <c r="AD134" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE134" s="29">
+        <v>0.290891599</v>
+      </c>
+      <c r="AF134" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG134" s="72"/>
+      <c r="AH134" s="73"/>
+      <c r="AI134" s="73"/>
+      <c r="AJ134" s="73"/>
+      <c r="AK134" s="73"/>
+    </row>
+    <row r="135" spans="1:37">
+      <c r="A135" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="B135" s="27">
+        <v>0.64851349599999997</v>
+      </c>
+      <c r="C135" s="27">
+        <v>0.74857399999999996</v>
+      </c>
+      <c r="D135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E135" s="27">
+        <v>0.40296756099999997</v>
+      </c>
+      <c r="F135" s="27">
+        <v>0.68442800000000004</v>
+      </c>
+      <c r="G135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H135" s="27">
+        <v>1.203668293</v>
+      </c>
+      <c r="I135" s="27">
+        <v>3.6802139999999999</v>
+      </c>
+      <c r="J135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K135" s="27">
+        <v>5</v>
+      </c>
+      <c r="L135" s="27">
+        <v>0</v>
+      </c>
+      <c r="M135" s="28">
+        <v>0</v>
+      </c>
+      <c r="N135" s="27">
+        <v>3</v>
+      </c>
+      <c r="O135" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="P135" s="28">
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="Q135" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="R135" s="27">
+        <v>7.9070056E-2</v>
+      </c>
+      <c r="S135" s="27">
+        <v>8.5931357999999999E-2</v>
+      </c>
+      <c r="T135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U135" s="27">
+        <v>0.18361965399999999</v>
+      </c>
+      <c r="V135" s="27">
+        <v>0.238047333</v>
+      </c>
+      <c r="W135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="X135" s="27">
+        <v>1.6689872809999999</v>
+      </c>
+      <c r="Y135" s="27">
+        <v>1.2619925599999999</v>
+      </c>
+      <c r="Z135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA135" s="31">
+        <v>3.0188415999999999E-2</v>
+      </c>
+      <c r="AB135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC135" s="31">
+        <v>2.8865814E-2</v>
+      </c>
+      <c r="AD135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE135" s="31">
+        <v>6.0442639999999997E-3</v>
+      </c>
+      <c r="AF135" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG135" s="72"/>
+      <c r="AH135" s="73"/>
+      <c r="AI135" s="73"/>
+      <c r="AJ135" s="73"/>
+      <c r="AK135" s="73"/>
+    </row>
+    <row r="136" spans="1:37">
+      <c r="A136" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="B136" s="27">
+        <v>0.78560815299999998</v>
+      </c>
+      <c r="C136" s="27">
+        <v>0.85131000000000001</v>
+      </c>
+      <c r="D136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E136" s="27">
+        <v>0.73232978900000001</v>
+      </c>
+      <c r="F136" s="27">
+        <v>0.94977999999999996</v>
+      </c>
+      <c r="G136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H136" s="27">
+        <v>3.7893785750000002</v>
+      </c>
+      <c r="I136" s="27">
+        <v>5.4068100000000001</v>
+      </c>
+      <c r="J136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K136" s="27">
+        <v>1</v>
+      </c>
+      <c r="L136" s="27">
+        <v>0</v>
+      </c>
+      <c r="M136" s="28">
+        <v>0</v>
+      </c>
+      <c r="N136" s="27">
+        <v>1</v>
+      </c>
+      <c r="O136" s="28">
+        <v>1</v>
+      </c>
+      <c r="P136" s="28">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="Q136" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="R136" s="27">
+        <v>7.3000581999999994E-2</v>
+      </c>
+      <c r="S136" s="27">
+        <v>0</v>
+      </c>
+      <c r="T136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U136" s="27">
+        <v>0.25551343799999998</v>
+      </c>
+      <c r="V136" s="27">
+        <v>0</v>
+      </c>
+      <c r="W136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="X136" s="27">
+        <v>1.933964996</v>
+      </c>
+      <c r="Y136" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF136" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG136" s="72"/>
+      <c r="AH136" s="73"/>
+      <c r="AI136" s="73"/>
+      <c r="AJ136" s="73"/>
+      <c r="AK136" s="73"/>
+    </row>
+    <row r="137" spans="1:37">
+      <c r="A137" s="72" t="s">
+        <v>190</v>
+      </c>
+      <c r="B137" s="27">
+        <v>0.690646341</v>
+      </c>
+      <c r="C137" s="27">
+        <v>0.69647000000000003</v>
+      </c>
+      <c r="D137" s="27">
+        <v>0.62116000000000005</v>
+      </c>
+      <c r="E137" s="27">
+        <v>0.50228403499999996</v>
+      </c>
+      <c r="F137" s="27">
+        <v>0.51130333299999997</v>
+      </c>
+      <c r="G137" s="27">
+        <v>0.34387000000000001</v>
+      </c>
+      <c r="H137" s="27">
+        <v>1.535493835</v>
+      </c>
+      <c r="I137" s="29">
+        <v>1.0808866669999999</v>
+      </c>
+      <c r="J137" s="27">
+        <v>0.90385000000000004</v>
+      </c>
+      <c r="K137" s="27">
+        <v>4</v>
+      </c>
+      <c r="L137" s="27">
+        <v>1</v>
+      </c>
+      <c r="M137" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="N137" s="27">
+        <v>0</v>
+      </c>
+      <c r="O137" s="28">
+        <v>0</v>
+      </c>
+      <c r="P137" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="R137" s="27">
+        <v>8.2697382E-2</v>
+      </c>
+      <c r="S137" s="27">
+        <v>1.3493028000000001E-2</v>
+      </c>
+      <c r="T137" s="27">
+        <v>0</v>
+      </c>
+      <c r="U137" s="27">
+        <v>0.19537342699999999</v>
+      </c>
+      <c r="V137" s="27">
+        <v>0.122610836</v>
+      </c>
+      <c r="W137" s="27">
+        <v>0</v>
+      </c>
+      <c r="X137" s="27">
+        <v>2.1146824080000002</v>
+      </c>
+      <c r="Y137" s="27">
+        <v>1.980723891</v>
+      </c>
+      <c r="Z137" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA137" s="29">
+        <v>0.28851396600000001</v>
+      </c>
+      <c r="AB137" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC137" s="29">
+        <v>0.45555422699999998</v>
+      </c>
+      <c r="AD137" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE137" s="36">
+        <v>0.36522911000000002</v>
+      </c>
+      <c r="AF137" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG137" s="72"/>
+      <c r="AH137" s="73"/>
+      <c r="AI137" s="73"/>
+      <c r="AJ137" s="73"/>
+      <c r="AK137" s="73"/>
+    </row>
+    <row r="138" spans="1:37">
+      <c r="A138" s="75" t="s">
+        <v>191</v>
+      </c>
+      <c r="B138" s="39">
+        <v>0.69764294100000002</v>
+      </c>
+      <c r="C138" s="41">
+        <v>0.46253</v>
+      </c>
+      <c r="D138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E138" s="39">
+        <v>0.54129764700000005</v>
+      </c>
+      <c r="F138" s="41">
+        <v>0.28656999999999999</v>
+      </c>
+      <c r="G138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H138" s="39">
+        <v>2.4332564310000002</v>
+      </c>
+      <c r="I138" s="39">
+        <v>2.5168300000000001</v>
+      </c>
+      <c r="J138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="K138" s="39">
+        <v>1</v>
+      </c>
+      <c r="L138" s="39">
+        <v>0</v>
+      </c>
+      <c r="M138" s="40">
+        <v>0</v>
+      </c>
+      <c r="N138" s="39">
+        <v>0</v>
+      </c>
+      <c r="O138" s="40">
+        <v>0</v>
+      </c>
+      <c r="P138" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="R138" s="39">
+        <v>9.8110669999999997E-2</v>
+      </c>
+      <c r="S138" s="39">
+        <v>0</v>
+      </c>
+      <c r="T138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="U138" s="39">
+        <v>0.220871915</v>
+      </c>
+      <c r="V138" s="39">
+        <v>0</v>
+      </c>
+      <c r="W138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="X138" s="39">
+        <v>1.85526561</v>
+      </c>
+      <c r="Y138" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG138" s="74"/>
+      <c r="AH138" s="73"/>
+      <c r="AI138" s="73"/>
+      <c r="AJ138" s="73"/>
+      <c r="AK138" s="73"/>
+    </row>
+    <row r="139" spans="1:37">
+      <c r="A139" s="72" t="s">
+        <v>192</v>
+      </c>
+      <c r="B139" s="27">
+        <v>0.71094695799999996</v>
+      </c>
+      <c r="C139" s="36">
+        <v>0.72791464299999997</v>
+      </c>
+      <c r="D139" s="27">
+        <v>0.73643999999999998</v>
+      </c>
+      <c r="E139" s="27">
+        <v>0.56389587299999999</v>
+      </c>
+      <c r="F139" s="27">
+        <v>0.58836785700000005</v>
+      </c>
+      <c r="G139" s="27">
+        <v>0.46006000000000002</v>
+      </c>
+      <c r="H139" s="27">
+        <v>2.4158732230000002</v>
+      </c>
+      <c r="I139" s="27">
+        <v>2.8403575000000001</v>
+      </c>
+      <c r="J139" s="27">
+        <v>1.9782500000000001</v>
+      </c>
+      <c r="K139" s="27">
+        <v>57</v>
+      </c>
+      <c r="L139" s="27">
+        <v>1</v>
+      </c>
+      <c r="M139" s="28">
+        <f>L139/K139</f>
+        <v>1.7543859649122806E-2</v>
+      </c>
+      <c r="N139" s="27">
+        <v>15</v>
+      </c>
+      <c r="O139" s="28">
+        <f>N139/K139</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="P139" s="28">
+        <v>8.43E-2</v>
+      </c>
+      <c r="Q139" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="R139" s="27">
+        <v>0.104845777</v>
+      </c>
+      <c r="S139" s="27">
+        <v>0.105318127</v>
+      </c>
+      <c r="T139" s="27">
+        <v>0</v>
+      </c>
+      <c r="U139" s="27">
+        <v>0.20766440999999999</v>
+      </c>
+      <c r="V139" s="27">
+        <v>0.175658798</v>
+      </c>
+      <c r="W139" s="27">
+        <v>0</v>
+      </c>
+      <c r="X139" s="27">
+        <v>1.4700698219999999</v>
+      </c>
+      <c r="Y139" s="27">
+        <v>1.0935225070000001</v>
+      </c>
+      <c r="Z139" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA139" s="29">
+        <v>0.12589409500000001</v>
+      </c>
+      <c r="AB139" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC139" s="29">
+        <v>0.16421408100000001</v>
+      </c>
+      <c r="AD139" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE139" s="31">
+        <v>4.5257250000000004E-3</v>
+      </c>
+      <c r="AF139" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG139" s="72"/>
+      <c r="AH139" s="73"/>
+      <c r="AI139" s="73"/>
+      <c r="AJ139" s="73"/>
+      <c r="AK139" s="73"/>
+    </row>
+    <row r="140" spans="1:37">
+      <c r="A140" s="72" t="s">
+        <v>193</v>
+      </c>
+      <c r="B140" s="27">
+        <v>0.70279288399999995</v>
+      </c>
+      <c r="C140" s="27">
+        <v>0.72143000000000002</v>
+      </c>
+      <c r="D140" s="27">
+        <v>0.671072</v>
+      </c>
+      <c r="E140" s="27">
+        <v>0.47054919699999997</v>
+      </c>
+      <c r="F140" s="27">
+        <v>0.49304999999999999</v>
+      </c>
+      <c r="G140" s="27">
+        <v>0.381276</v>
+      </c>
+      <c r="H140" s="27">
+        <v>1.7732698920000001</v>
+      </c>
+      <c r="I140" s="29">
+        <v>1.06755</v>
+      </c>
+      <c r="J140" s="27">
+        <v>0.15391199999999999</v>
+      </c>
+      <c r="K140" s="27">
+        <v>6</v>
+      </c>
+      <c r="L140" s="27">
+        <v>5</v>
+      </c>
+      <c r="M140" s="28">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="N140" s="27">
+        <v>0</v>
+      </c>
+      <c r="O140" s="28">
+        <v>0</v>
+      </c>
+      <c r="P140" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q140" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="R140" s="27">
+        <v>7.2158782000000005E-2</v>
+      </c>
+      <c r="S140" s="27">
+        <v>0</v>
+      </c>
+      <c r="T140" s="27">
+        <v>1.8038063999999999E-2</v>
+      </c>
+      <c r="U140" s="27">
+        <v>0.20726910000000001</v>
+      </c>
+      <c r="V140" s="27">
+        <v>0</v>
+      </c>
+      <c r="W140" s="27">
+        <v>0.108947232</v>
+      </c>
+      <c r="X140" s="27">
+        <v>1.733775938</v>
+      </c>
+      <c r="Y140" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z140" s="27">
+        <v>1.415315935</v>
+      </c>
+      <c r="AA140" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB140" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC140" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD140" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE140" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF140" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG140" s="72"/>
+      <c r="AH140" s="73"/>
+      <c r="AI140" s="73"/>
+      <c r="AJ140" s="73"/>
+      <c r="AK140" s="73"/>
+    </row>
+    <row r="141" spans="1:37">
+      <c r="A141" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="B141" s="27">
+        <v>0.78493934799999998</v>
+      </c>
+      <c r="C141" s="27">
+        <v>0.81992571400000003</v>
+      </c>
+      <c r="D141" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E141" s="27">
+        <v>0.70997175000000001</v>
+      </c>
+      <c r="F141" s="27">
+        <v>0.820974286</v>
+      </c>
+      <c r="G141" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H141" s="27">
+        <v>0.78493934799999998</v>
+      </c>
+      <c r="I141" s="27">
+        <v>0.81992571400000003</v>
+      </c>
+      <c r="J141" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="K141" s="27">
+        <v>14</v>
+      </c>
+      <c r="L141" s="27">
+        <v>0</v>
+      </c>
+      <c r="M141" s="28">
+        <v>0</v>
+      </c>
+      <c r="N141" s="27">
+        <v>12</v>
+      </c>
+      <c r="O141" s="28">
+        <v>0.85709999999999997</v>
+      </c>
+      <c r="P141" s="28">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="Q141" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="R141" s="27">
+        <v>6.6046658999999994E-2</v>
+      </c>
+      <c r="S141" s="27">
+        <v>4.0566029000000003E-2</v>
+      </c>
+      <c r="T141" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="U141" s="27">
+        <v>0.25603424800000002</v>
+      </c>
+      <c r="V141" s="27">
+        <v>0.204070845</v>
+      </c>
+      <c r="W141" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="X141" s="27">
+        <v>6.6046658999999994E-2</v>
+      </c>
+      <c r="Y141" s="27">
+        <v>4.0566029000000003E-2</v>
+      </c>
+      <c r="Z141" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA141" s="31">
+        <v>3.4083590000000001E-3</v>
+      </c>
+      <c r="AB141" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC141" s="31">
+        <v>3.1704639E-2</v>
+      </c>
+      <c r="AD141" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE141" s="31">
+        <v>3.4083590000000001E-3</v>
+      </c>
+      <c r="AF141" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG141" s="72"/>
+      <c r="AH141" s="73"/>
+      <c r="AI141" s="73"/>
+      <c r="AJ141" s="73"/>
+      <c r="AK141" s="73"/>
+    </row>
+    <row r="142" spans="1:37">
+      <c r="A142" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="B142" s="27">
+        <v>0.78739871900000002</v>
+      </c>
+      <c r="C142" s="27">
+        <v>0.85609999999999997</v>
+      </c>
+      <c r="D142" s="27">
+        <v>0.81242000000000003</v>
+      </c>
+      <c r="E142" s="27">
+        <v>0.784461144</v>
+      </c>
+      <c r="F142" s="36">
+        <v>0.95118999999999998</v>
+      </c>
+      <c r="G142" s="27">
+        <v>0.99997000000000003</v>
+      </c>
+      <c r="H142" s="27">
+        <v>4.1699262399999997</v>
+      </c>
+      <c r="I142" s="27">
+        <v>5.3309100000000003</v>
+      </c>
+      <c r="J142" s="27">
+        <v>4.5</v>
+      </c>
+      <c r="K142" s="27">
+        <v>2</v>
+      </c>
+      <c r="L142" s="27">
+        <v>1</v>
+      </c>
+      <c r="M142" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="N142" s="27">
+        <v>1</v>
+      </c>
+      <c r="O142" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="P142" s="28">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="Q142" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="R142" s="27">
+        <v>9.7746701000000005E-2</v>
+      </c>
+      <c r="S142" s="27">
+        <v>0</v>
+      </c>
+      <c r="T142" s="27">
+        <v>0</v>
+      </c>
+      <c r="U142" s="27">
+        <v>0.28764371399999999</v>
+      </c>
+      <c r="V142" s="27">
+        <v>0</v>
+      </c>
+      <c r="W142" s="27">
+        <v>0</v>
+      </c>
+      <c r="X142" s="27">
+        <v>1.828029742</v>
+      </c>
+      <c r="Y142" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z142" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA142" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB142" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC142" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD142" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE142" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF142" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG142" s="72"/>
+      <c r="AH142" s="73"/>
+      <c r="AI142" s="73"/>
+      <c r="AJ142" s="73"/>
+      <c r="AK142" s="73"/>
+    </row>
+    <row r="143" spans="1:37">
+      <c r="A143" s="72" t="s">
+        <v>196</v>
+      </c>
+      <c r="B143" s="27">
+        <v>0.68898657799999996</v>
+      </c>
+      <c r="C143" s="27">
+        <v>0.78777399999999997</v>
+      </c>
+      <c r="D143" s="27">
+        <v>0.69610000000000005</v>
+      </c>
+      <c r="E143" s="27">
+        <v>0.52620514299999999</v>
+      </c>
+      <c r="F143" s="27">
+        <v>0.75548800000000005</v>
+      </c>
+      <c r="G143" s="27">
+        <v>0.52274833300000001</v>
+      </c>
+      <c r="H143" s="27">
+        <v>2.2765291300000001</v>
+      </c>
+      <c r="I143" s="27">
+        <v>4.3944330000000003</v>
+      </c>
+      <c r="J143" s="27">
+        <v>2.3231850000000001</v>
+      </c>
+      <c r="K143" s="27">
+        <v>16</v>
+      </c>
+      <c r="L143" s="27">
+        <v>6</v>
+      </c>
+      <c r="M143" s="28">
+        <v>0.375</v>
+      </c>
+      <c r="N143" s="27">
+        <v>6</v>
+      </c>
+      <c r="O143" s="28">
+        <v>0.375</v>
+      </c>
+      <c r="P143" s="28">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="Q143" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="R143" s="27">
+        <v>0.106964355</v>
+      </c>
+      <c r="S143" s="27">
+        <v>4.3778414000000002E-2</v>
+      </c>
+      <c r="T143" s="27">
+        <v>5.9043984000000001E-2</v>
+      </c>
+      <c r="U143" s="27">
+        <v>0.23387204</v>
+      </c>
+      <c r="V143" s="27">
+        <v>0.14526349999999999</v>
+      </c>
+      <c r="W143" s="27">
+        <v>0.13268808200000001</v>
+      </c>
+      <c r="X143" s="27">
+        <v>2.0023318259999998</v>
+      </c>
+      <c r="Y143" s="27">
+        <v>1.179108643</v>
+      </c>
+      <c r="Z143" s="27">
+        <v>1.205493082</v>
+      </c>
+      <c r="AA143" s="38">
+        <v>3.4022200000000001E-5</v>
+      </c>
+      <c r="AB143" s="31">
+        <v>1.0761997000000001E-2</v>
+      </c>
+      <c r="AC143" s="31">
+        <v>4.0748999999999999E-4</v>
+      </c>
+      <c r="AD143" s="31">
+        <v>1.1015107E-2</v>
+      </c>
+      <c r="AE143" s="31">
+        <v>1.6697899999999999E-4</v>
+      </c>
+      <c r="AF143" s="31">
+        <v>1.0113716E-2</v>
+      </c>
+      <c r="AG143" s="72"/>
+      <c r="AH143" s="73"/>
+      <c r="AI143" s="73"/>
+      <c r="AJ143" s="73"/>
+      <c r="AK143" s="73"/>
+    </row>
+    <row r="144" spans="1:37">
+      <c r="A144" s="72" t="s">
+        <v>197</v>
+      </c>
+      <c r="B144" s="27">
+        <v>0.68323228700000005</v>
+      </c>
+      <c r="C144" s="27">
+        <v>0.69768333299999996</v>
+      </c>
+      <c r="D144" s="27">
+        <v>0.61380999999999997</v>
+      </c>
+      <c r="E144" s="27">
+        <v>0.46978498299999999</v>
+      </c>
+      <c r="F144" s="27">
+        <v>0.49180000000000001</v>
+      </c>
+      <c r="G144" s="27">
+        <v>0.35124</v>
+      </c>
+      <c r="H144" s="27">
+        <v>1.883738259</v>
+      </c>
+      <c r="I144" s="29">
+        <v>0.86336666699999998</v>
+      </c>
+      <c r="J144" s="27">
+        <v>0.92598999999999998</v>
+      </c>
+      <c r="K144" s="27">
+        <v>4</v>
+      </c>
+      <c r="L144" s="27">
+        <v>1</v>
+      </c>
+      <c r="M144" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="N144" s="27">
+        <v>1</v>
+      </c>
+      <c r="O144" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="P144" s="28">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="Q144" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="R144" s="27">
+        <v>8.4595136000000001E-2</v>
+      </c>
+      <c r="S144" s="27">
+        <v>6.8337942999999998E-2</v>
+      </c>
+      <c r="T144" s="27">
+        <v>0</v>
+      </c>
+      <c r="U144" s="27">
+        <v>0.21958671699999999</v>
+      </c>
+      <c r="V144" s="27">
+        <v>0.241167667</v>
+      </c>
+      <c r="W144" s="27">
+        <v>0</v>
+      </c>
+      <c r="X144" s="27">
+        <v>2.0865303239999999</v>
+      </c>
+      <c r="Y144" s="27">
+        <v>1.8808509410000001</v>
+      </c>
+      <c r="Z144" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA144" s="29">
+        <v>0.374947117</v>
+      </c>
+      <c r="AB144" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC144" s="29">
+        <v>0.44452309800000001</v>
+      </c>
+      <c r="AD144" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE144" s="36">
+        <v>0.22369719299999999</v>
+      </c>
+      <c r="AF144" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG144" s="72"/>
+      <c r="AH144" s="73"/>
+      <c r="AI144" s="73"/>
+      <c r="AJ144" s="73"/>
+      <c r="AK144" s="73"/>
+    </row>
+    <row r="145" spans="1:32">
+      <c r="A145" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B132" s="1">
-        <f>AVERAGE(B2:B131)</f>
-        <v>0.71114124153530234</v>
-      </c>
-      <c r="C132" s="1">
-        <f t="shared" ref="C132:AF132" si="4">AVERAGE(C2:C131)</f>
-        <v>0.74910127098068324</v>
-      </c>
-      <c r="D132" s="1">
+      <c r="B145" s="1">
+        <f>AVERAGE(B2:B144)</f>
+        <v>0.71199052844339494</v>
+      </c>
+      <c r="C145" s="1">
+        <f t="shared" ref="C145:AF145" si="4">AVERAGE(C2:C144)</f>
+        <v>0.74833488376452639</v>
+      </c>
+      <c r="D145" s="1">
         <f t="shared" si="4"/>
-        <v>0.65236670701101773</v>
-      </c>
-      <c r="E132" s="1">
+        <v>0.65768088275200554</v>
+      </c>
+      <c r="E145" s="1">
         <f t="shared" si="4"/>
-        <v>0.5739236453479668</v>
-      </c>
-      <c r="F132" s="1">
+        <v>0.57490398831611056</v>
+      </c>
+      <c r="F145" s="1">
         <f t="shared" si="4"/>
-        <v>0.67889740186094261</v>
-      </c>
-      <c r="G132" s="1">
+        <v>0.67705523332566242</v>
+      </c>
+      <c r="G145" s="1">
         <f t="shared" si="4"/>
-        <v>0.42656095103286656</v>
-      </c>
-      <c r="H132" s="1">
+        <v>0.43613618463218984</v>
+      </c>
+      <c r="H145" s="1">
         <f t="shared" si="4"/>
-        <v>2.554916510456688</v>
-      </c>
-      <c r="I132" s="1">
+        <v>2.5431308871050198</v>
+      </c>
+      <c r="I145" s="1">
         <f t="shared" si="4"/>
-        <v>3.4286562937363221</v>
-      </c>
-      <c r="J132" s="1">
+        <v>3.3872443994688619</v>
+      </c>
+      <c r="J145" s="1">
         <f t="shared" si="4"/>
-        <v>1.4125324503979457</v>
-      </c>
-      <c r="K132" s="1">
+        <v>1.4800652181056493</v>
+      </c>
+      <c r="K145" s="1">
         <f t="shared" si="4"/>
-        <v>12.108527131782946</v>
-      </c>
-      <c r="L132" s="1">
+        <v>11.915492957746478</v>
+      </c>
+      <c r="L145" s="1">
         <f t="shared" si="4"/>
-        <v>2.3410852713178296</v>
-      </c>
-      <c r="M132" s="1">
+        <v>2.2464788732394365</v>
+      </c>
+      <c r="M145" s="1">
         <f t="shared" si="4"/>
-        <v>0.21353817863823346</v>
-      </c>
-      <c r="N132" s="1">
+        <v>0.21221837674868013</v>
+      </c>
+      <c r="N145" s="1">
         <f t="shared" si="4"/>
-        <v>5.6111111111111107</v>
-      </c>
-      <c r="O132" s="1">
+        <v>5.4316546762589928</v>
+      </c>
+      <c r="O145" s="1">
         <f t="shared" si="4"/>
-        <v>0.37209166588538151</v>
-      </c>
-      <c r="P132" s="1">
+        <v>0.37262955249133034</v>
+      </c>
+      <c r="P145" s="1">
         <f t="shared" si="4"/>
-        <v>3.4012060891914372E-2</v>
-      </c>
-      <c r="Q132" s="1" t="e">
+        <v>3.2357695484756914E-2</v>
+      </c>
+      <c r="Q145" s="1" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R132" s="1">
+      <c r="R145" s="1">
         <f t="shared" si="4"/>
-        <v>9.2780022643792592E-2</v>
-      </c>
-      <c r="S132" s="1">
+        <v>9.262046797922005E-2</v>
+      </c>
+      <c r="S145" s="1">
         <f t="shared" si="4"/>
-        <v>5.4408296838096101E-2</v>
-      </c>
-      <c r="T132" s="1">
+        <v>5.3736173192267159E-2</v>
+      </c>
+      <c r="T145" s="1">
         <f t="shared" si="4"/>
-        <v>5.0577034778534674E-2</v>
-      </c>
-      <c r="U132" s="1">
+        <v>4.7055161335219857E-2</v>
+      </c>
+      <c r="U145" s="1">
         <f t="shared" si="4"/>
-        <v>0.21902884759413357</v>
-      </c>
-      <c r="V132" s="1">
+        <v>0.21995091145523404</v>
+      </c>
+      <c r="V145" s="1">
         <f t="shared" si="4"/>
-        <v>0.15292295642523213</v>
-      </c>
-      <c r="W132" s="1">
+        <v>0.15168975024081097</v>
+      </c>
+      <c r="W145" s="1">
         <f t="shared" si="4"/>
-        <v>0.1164723412387554</v>
-      </c>
-      <c r="X132" s="1">
+        <v>0.10905144429348611</v>
+      </c>
+      <c r="X145" s="1">
         <f t="shared" si="4"/>
-        <v>1.8027187377548772</v>
-      </c>
-      <c r="Y132" s="1">
+        <v>1.7895261063970362</v>
+      </c>
+      <c r="Y145" s="1">
         <f t="shared" si="4"/>
-        <v>1.3132783175251195</v>
-      </c>
-      <c r="Z132" s="1">
+        <v>1.2763692356173426</v>
+      </c>
+      <c r="Z145" s="1">
         <f t="shared" si="4"/>
-        <v>0.91450613607344433</v>
-      </c>
-      <c r="AA132" s="1">
+        <v>0.86401968369078241</v>
+      </c>
+      <c r="AA145" s="1">
         <f t="shared" si="4"/>
-        <v>0.11594995315147363</v>
-      </c>
-      <c r="AB132" s="1">
+        <v>0.1179739746670392</v>
+      </c>
+      <c r="AB145" s="1">
         <f t="shared" si="4"/>
-        <v>0.16450279123065414</v>
-      </c>
-      <c r="AC132" s="1">
+        <v>0.16170750406282405</v>
+      </c>
+      <c r="AC145" s="1">
         <f t="shared" si="4"/>
-        <v>0.12407446916269681</v>
-      </c>
-      <c r="AD132" s="1">
+        <v>0.13113853962486402</v>
+      </c>
+      <c r="AD145" s="1">
         <f t="shared" si="4"/>
-        <v>0.13769051464866897</v>
-      </c>
-      <c r="AE132" s="1">
+        <v>0.13538732541869319</v>
+      </c>
+      <c r="AE145" s="1">
         <f t="shared" si="4"/>
-        <v>0.1248506642345445</v>
-      </c>
-      <c r="AF132" s="1">
+        <v>0.12697566936919788</v>
+      </c>
+      <c r="AF145" s="1">
         <f t="shared" si="4"/>
-        <v>0.12504704126638</v>
+        <v>0.12295734444335492</v>
       </c>
     </row>
-    <row r="133" spans="1:37">
-      <c r="A133" s="1" t="s">
+    <row r="146" spans="1:32">
+      <c r="A146" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B133" s="1">
-        <f>STDEV(B2:B131)</f>
-        <v>5.7245678289866327E-2</v>
-      </c>
-      <c r="C133" s="1">
-        <f t="shared" ref="C133:AF133" si="5">STDEV(C2:C131)</f>
-        <v>8.3885508743371487E-2</v>
-      </c>
-      <c r="D133" s="1">
+      <c r="B146" s="1">
+        <f>STDEV(B2:B144)</f>
+        <v>5.6037517892706133E-2</v>
+      </c>
+      <c r="C146" s="1">
+        <f t="shared" ref="C146:AF146" si="5">STDEV(C2:C144)</f>
+        <v>8.5264883158607183E-2</v>
+      </c>
+      <c r="D146" s="1">
         <f t="shared" si="5"/>
-        <v>0.11402773320110693</v>
-      </c>
-      <c r="E133" s="1">
+        <v>0.11229934379134589</v>
+      </c>
+      <c r="E146" s="1">
         <f t="shared" si="5"/>
-        <v>0.11186211451619221</v>
-      </c>
-      <c r="F133" s="1">
+        <v>0.11179114771534435</v>
+      </c>
+      <c r="F146" s="1">
         <f t="shared" si="5"/>
-        <v>0.15397833742227016</v>
-      </c>
-      <c r="G133" s="1">
+        <v>0.15783300745795287</v>
+      </c>
+      <c r="G146" s="1">
         <f t="shared" si="5"/>
-        <v>0.18678734842226574</v>
-      </c>
-      <c r="H133" s="1">
+        <v>0.1927517278804903</v>
+      </c>
+      <c r="H146" s="1">
         <f t="shared" si="5"/>
-        <v>0.89535938592255848</v>
-      </c>
-      <c r="I133" s="1">
+        <v>0.90246574133062107</v>
+      </c>
+      <c r="I146" s="1">
         <f t="shared" si="5"/>
-        <v>1.2559884315684069</v>
-      </c>
-      <c r="J133" s="1">
+        <v>1.2988372313215191</v>
+      </c>
+      <c r="J146" s="1">
         <f t="shared" si="5"/>
-        <v>1.4905559699281381</v>
-      </c>
-      <c r="K133" s="1">
+        <v>1.5125820298945782</v>
+      </c>
+      <c r="K146" s="1">
         <f t="shared" si="5"/>
-        <v>14.111852459721979</v>
-      </c>
-      <c r="L133" s="1">
+        <v>14.140878300762344</v>
+      </c>
+      <c r="L146" s="1">
         <f t="shared" si="5"/>
-        <v>3.9794317355603042</v>
-      </c>
-      <c r="M133" s="1">
+        <v>3.8448392596017076</v>
+      </c>
+      <c r="M146" s="1">
         <f t="shared" si="5"/>
-        <v>0.25141860793720699</v>
-      </c>
-      <c r="N133" s="1">
+        <v>0.25057687080466018</v>
+      </c>
+      <c r="N146" s="1">
         <f t="shared" si="5"/>
-        <v>8.4729897648678634</v>
-      </c>
-      <c r="O133" s="1">
+        <v>8.2127952131549407</v>
+      </c>
+      <c r="O146" s="1">
         <f t="shared" si="5"/>
-        <v>0.29487103542785964</v>
-      </c>
-      <c r="P133" s="1">
+        <v>0.29718295264914157</v>
+      </c>
+      <c r="P146" s="1">
         <f t="shared" si="5"/>
-        <v>5.1792965742672954E-2</v>
-      </c>
-      <c r="Q133" s="1" t="e">
+        <v>5.0155932579908614E-2</v>
+      </c>
+      <c r="Q146" s="1" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R133" s="1">
+      <c r="R146" s="1">
         <f t="shared" si="5"/>
-        <v>3.0712122208433081E-2</v>
-      </c>
-      <c r="S133" s="1">
+        <v>2.9609800962308228E-2</v>
+      </c>
+      <c r="S146" s="1">
         <f t="shared" si="5"/>
-        <v>3.669176472197281E-2</v>
-      </c>
-      <c r="T133" s="1">
+        <v>3.7260191085193933E-2</v>
+      </c>
+      <c r="T146" s="1">
         <f t="shared" si="5"/>
-        <v>5.4783027792466812E-2</v>
-      </c>
-      <c r="U133" s="1">
+        <v>5.3914615434804032E-2</v>
+      </c>
+      <c r="U146" s="1">
         <f t="shared" si="5"/>
-        <v>3.6346988832474204E-2</v>
-      </c>
-      <c r="V133" s="1">
+        <v>3.5872079699091397E-2</v>
+      </c>
+      <c r="V146" s="1">
         <f t="shared" si="5"/>
-        <v>8.1281241237794191E-2</v>
-      </c>
-      <c r="W133" s="1">
+        <v>8.4068684064441984E-2</v>
+      </c>
+      <c r="W146" s="1">
         <f t="shared" si="5"/>
-        <v>0.11316202924556737</v>
-      </c>
-      <c r="X133" s="1">
+        <v>0.11191354876218651</v>
+      </c>
+      <c r="X146" s="1">
         <f t="shared" si="5"/>
-        <v>0.24030880315062214</v>
-      </c>
-      <c r="Y133" s="1">
+        <v>0.27808460053734108</v>
+      </c>
+      <c r="Y146" s="1">
         <f t="shared" si="5"/>
-        <v>0.71225615993562108</v>
-      </c>
-      <c r="Z133" s="1">
+        <v>0.7276064194926477</v>
+      </c>
+      <c r="Z146" s="1">
         <f t="shared" si="5"/>
-        <v>0.82519830483503953</v>
-      </c>
-      <c r="AA133" s="1">
+        <v>0.8230137818726746</v>
+      </c>
+      <c r="AA146" s="1">
         <f t="shared" si="5"/>
-        <v>0.13815528450612202</v>
-      </c>
-      <c r="AB133" s="1">
+        <v>0.13916716019692876</v>
+      </c>
+      <c r="AB146" s="1">
         <f t="shared" si="5"/>
-        <v>0.13036996193202705</v>
-      </c>
-      <c r="AC133" s="1">
+        <v>0.13081028188802818</v>
+      </c>
+      <c r="AC146" s="1">
         <f t="shared" si="5"/>
-        <v>0.14199005547911267</v>
-      </c>
-      <c r="AD133" s="1">
+        <v>0.14841461816118801</v>
+      </c>
+      <c r="AD146" s="1">
         <f t="shared" si="5"/>
-        <v>0.12296703134322612</v>
-      </c>
-      <c r="AE133" s="1">
+        <v>0.12301476226745164</v>
+      </c>
+      <c r="AE146" s="1">
         <f t="shared" si="5"/>
-        <v>0.13966078763946979</v>
-      </c>
-      <c r="AF133" s="1">
+        <v>0.14288131326497858</v>
+      </c>
+      <c r="AF146" s="1">
         <f t="shared" si="5"/>
-        <v>9.9476176175361752E-2</v>
+        <v>9.9761892789143061E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:37">
-      <c r="Z134" s="1" t="s">
+    <row r="147" spans="1:32">
+      <c r="Z147" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="AA134" s="69">
-        <v>3.1909309999999997E-5</v>
-      </c>
-      <c r="AB134" s="70">
-        <v>2.7527450000000001E-10</v>
-      </c>
-      <c r="AC134" s="70">
-        <v>6.0635810000000002E-9</v>
-      </c>
-      <c r="AD134" s="70">
-        <v>4.510934E-18</v>
-      </c>
-      <c r="AE134" s="70">
-        <v>2.7673040000000002E-9</v>
-      </c>
-      <c r="AF134" s="70">
-        <v>6.3215010000000001E-18</v>
+      <c r="AA147" s="69">
+        <v>2.937831E-5</v>
+      </c>
+      <c r="AB147" s="70">
+        <v>3.4210120000000001E-10</v>
+      </c>
+      <c r="AC147" s="70">
+        <v>4.0273170000000004E-9</v>
+      </c>
+      <c r="AD147" s="70">
+        <v>9.2189080000000002E-18</v>
+      </c>
+      <c r="AE147" s="70">
+        <v>2.954396E-9</v>
+      </c>
+      <c r="AF147" s="70">
+        <v>1.4003720000000001E-17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>